<commit_message>
Updated to show queries
</commit_message>
<xml_diff>
--- a/2021-01-31/Meta Taxonomy.xlsx
+++ b/2021-01-31/Meta Taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Documents/GitHub/US-GAAP-MetaModel/2021-01-31/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B90327-A764-244E-A73E-C3441B6100FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C4D68-B301-C143-96A2-6C4120EA381A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="1160" windowWidth="35840" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7600" yWindow="2120" windowWidth="35840" windowHeight="20660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="presentation" sheetId="1" r:id="rId1"/>
@@ -758,11 +758,11 @@
       <sheetName val="DTS"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
-        <row r="26">
-          <cell r="F26" t="str">
+        <row r="27">
+          <cell r="F27" t="str">
             <v>000001 - Meta - MetaModel of US GAAP Taxonomy</v>
           </cell>
         </row>
@@ -1074,8 +1074,8 @@
   </sheetPr>
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1090,7 +1090,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1">
       <c r="A1" s="31" t="str">
-        <f>[1]DTS!F26</f>
+        <f>[1]DTS!F27</f>
         <v>000001 - Meta - MetaModel of US GAAP Taxonomy</v>
       </c>
       <c r="B1" s="1"/>
@@ -1945,8 +1945,8 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>